<commit_message>
added jokes in the database
Not my jokes because I only have only good jokes. the teachers may not like that one

why did the rooster cross the road?
He was a massive cock
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CFD475-BE78-4AB3-BFC0-E8D74E0CA63D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB89AEF-8C9C-40CE-BC33-176419161CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,64 +20,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>term 1</t>
-  </si>
-  <si>
-    <t>term 2</t>
-  </si>
-  <si>
-    <t>term 3</t>
-  </si>
-  <si>
-    <t>term 4</t>
-  </si>
-  <si>
-    <t>term 5</t>
-  </si>
-  <si>
-    <t>term 6</t>
-  </si>
-  <si>
-    <t>term 7</t>
-  </si>
-  <si>
-    <t>def 2</t>
-  </si>
-  <si>
-    <t>def 1</t>
-  </si>
-  <si>
-    <t>def 3</t>
-  </si>
-  <si>
-    <t>def 4</t>
-  </si>
-  <si>
-    <t>def 5</t>
-  </si>
-  <si>
-    <t>def 6</t>
-  </si>
-  <si>
-    <t>def 7</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TERMS</t>
   </si>
   <si>
     <t>DEF</t>
+  </si>
+  <si>
+    <t>Did you hear about the claustrophobic astronaut?</t>
+  </si>
+  <si>
+    <t>He just needed a little space</t>
+  </si>
+  <si>
+    <t>Did you hear about the guy who stole a calendar?</t>
+  </si>
+  <si>
+    <t>He got 12 months; they say his days are numbered.</t>
+  </si>
+  <si>
+    <t>I used to be addicted to soap,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> but I’m clean now.</t>
+  </si>
+  <si>
+    <t>I’m terrified of elevators</t>
+  </si>
+  <si>
+    <t>so I’m going to start taking steps to avoid them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did you hear about the mathematician who’s afraid of negative numbers? </t>
+  </si>
+  <si>
+    <t>He’ll stop at nothing to avoid them.</t>
+  </si>
+  <si>
+    <t>Why is that picture in jail?</t>
+  </si>
+  <si>
+    <t>Because it was framed</t>
+  </si>
+  <si>
+    <t>What do you call a sleeping dinosaur?</t>
+  </si>
+  <si>
+    <t>Dino snore</t>
+  </si>
+  <si>
+    <t>What is a link you can't click on</t>
+  </si>
+  <si>
+    <t>https://www.stylecraze.com/articles/jokes-to-tell-your-friends/#dumb-jokes-to-tell-your-friends</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,13 +114,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,55 +402,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -441,21 +460,32 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" location="dumb-jokes-to-tell-your-friends" xr:uid="{4727B1ED-38A2-4C7C-8D97-B94606E54E8B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>